<commit_message>
add table:number of components
Former-commit-id: d58a4477116e21fd78ae355e7fe1014ad38bcb9c
</commit_message>
<xml_diff>
--- a/note/SIPLIB_timeline.xlsx
+++ b/note/SIPLIB_timeline.xlsx
@@ -12,6 +12,9 @@
     <sheet name="timeline_v2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="timeline_v3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">timeline_v3!$A$1:$H$13</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t xml:space="preserve">Final expected 
 output</t>
@@ -232,16 +235,40 @@
     <t xml:space="preserve">1. SIPLIPv2 website (instance repository) (after submission0</t>
   </si>
   <si>
-    <t xml:space="preserve">Preprocess Julia codes (sizes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decide what to analyze: expected shape of figures, tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design of Experiment: Determine instances to generate, time limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run experiments on workstation (using Julia interface for storing result data)</t>
+    <t xml:space="preserve">Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-analysis on instances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size &amp; Complexity (e.g., #var, #constraints, %nonzeros, size increasing rate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint matrix (e.g., sparsity pattern, shape of the matrix)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which instances to generate for experiments? (decide by trial &amp; error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What to report for each instance?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to report? (graph, table, …)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write &amp; test codes for experiments (to run on Bebop or Blues)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run and monitor the experiments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrap-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post-analysis on the experiments</t>
   </si>
 </sst>
 </file>
@@ -252,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -325,8 +352,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +392,14 @@
         <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -552,6 +593,13 @@
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -581,7 +629,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -818,19 +866,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,7 +910,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -917,9 +977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>47520</xdr:colOff>
+      <xdr:colOff>47160</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -933,7 +993,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3255120" y="4662000"/>
-          <a:ext cx="8969040" cy="4882680"/>
+          <a:ext cx="8969400" cy="4882320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -955,7 +1015,7 @@
   </sheetPr>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1636,7 +1696,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2237,259 +2297,206 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="7.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="44"/>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="A3" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A4" s="62"/>
+      <c r="B4" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="64"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="60"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31"/>
-      <c r="B7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="64"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31"/>
-      <c r="B8" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="60"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48"/>
-      <c r="B9" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="60"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="60"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="60"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="60"/>
+      <c r="A12" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="48"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="62"/>
+      <c r="A13" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="63"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:L4"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A11"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="85" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>